<commit_message>
New projects and executables
New projects for simultaneity and automate transmission tree

New version of CovidSIMVL some bugs removed....
</commit_message>
<xml_diff>
--- a/CovidSIMVL/PROJECTS/2020.08 CovidSIMVL School+LTC+bar for TR006/Supporting/Mingle Factor by Universe Trials/MVp100i5allUmf10.xlsx
+++ b/CovidSIMVL/PROJECTS/2020.08 CovidSIMVL School+LTC+bar for TR006/Supporting/Mingle Factor by Universe Trials/MVp100i5allUmf10.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="68" windowWidth="26370" windowHeight="14828" firstSheet="6" activeTab="17"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="26376" windowHeight="14832" firstSheet="6" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="console.log" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="% increases" sheetId="16" r:id="rId17"/>
     <sheet name="theta" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -842,7 +843,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1289,7 +1290,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1421,7 +1422,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1483,11 +1483,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="274745984"/>
-        <c:axId val="274752640"/>
+        <c:axId val="336140544"/>
+        <c:axId val="336142336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="274745984"/>
+        <c:axId val="336140544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,7 +1496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="274752640"/>
+        <c:crossAx val="336142336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1504,7 +1504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274752640"/>
+        <c:axId val="336142336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="274745984"/>
+        <c:crossAx val="336140544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3705,454 +3705,454 @@
       <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -4170,7 +4170,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4185,7 +4185,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4200,7 +4200,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4215,7 +4215,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4230,7 +4230,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4245,7 +4245,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4260,102 +4260,102 @@
       <selection activeCell="H56" sqref="C39:H56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.53125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>223</v>
       </c>
@@ -4374,13 +4374,13 @@
       <selection activeCell="G25" sqref="G25:J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.53125" customWidth="1"/>
-    <col min="7" max="7" width="10.53125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>213</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>230</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>214</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>226</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>87</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>228</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>215</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>244</v>
       </c>
@@ -4444,12 +4444,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>216</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>229</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>217</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>224</v>
       </c>
@@ -4481,12 +4481,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>218</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>221</v>
       </c>
@@ -4502,22 +4502,22 @@
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>223</v>
       </c>
@@ -4536,9 +4536,9 @@
       <selection activeCell="C65" sqref="C65:M76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>247</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C5" s="19">
         <v>0.1</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C6" s="19">
         <v>0.2</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>67.666666666666671</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C7" s="19">
         <v>0.3</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>7.0333333333333332</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C8" s="19">
         <v>0.4</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>6.375</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" s="19">
         <v>0.5</v>
       </c>
@@ -4659,12 +4659,12 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -4685,7 +4685,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="19"/>
@@ -4706,7 +4706,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="19"/>
@@ -4714,7 +4714,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="19"/>
@@ -4722,7 +4722,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="19"/>
@@ -4733,7 +4733,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="19"/>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="19"/>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="19"/>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="19"/>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="19"/>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="19"/>
@@ -4851,7 +4851,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="19"/>
@@ -4862,7 +4862,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -4883,7 +4883,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H25" s="2">
         <v>346</v>
       </c>
@@ -4898,12 +4898,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H28" s="2">
         <v>164</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>218</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="21" t="s">
         <v>245</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>93.666666666666671</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="19">
         <v>0.1</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>104.75</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="19">
         <v>0.2</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>90.2</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="19">
         <v>0.3</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>12.588235294117647</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="19">
         <v>0.4</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="19">
         <v>0.5</v>
       </c>
@@ -5065,10 +5065,10 @@
         <v>9.5714285714285712</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="12"/>
@@ -5076,7 +5076,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="12"/>
@@ -5084,7 +5084,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="12"/>
@@ -5092,7 +5092,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="12"/>
@@ -5100,7 +5100,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="12"/>
@@ -5108,7 +5108,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>220</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>23</v>
       </c>
@@ -5159,11 +5159,11 @@
         <v>1</v>
       </c>
       <c r="L47" s="17">
-        <f>B47/K47</f>
+        <f t="shared" ref="L47:L56" si="6">B47/K47</f>
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>47</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>91</v>
       </c>
       <c r="I48" s="23">
-        <f t="shared" ref="I48:I51" si="6">H48/G48</f>
+        <f t="shared" ref="I48:I51" si="7">H48/G48</f>
         <v>30.333333333333332</v>
       </c>
       <c r="J48" s="1"/>
@@ -5194,11 +5194,11 @@
         <v>2</v>
       </c>
       <c r="L48" s="17">
-        <f>B48/K48</f>
+        <f t="shared" si="6"/>
         <v>23.5</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>91</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>93</v>
       </c>
       <c r="I49" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23.25</v>
       </c>
       <c r="J49" s="1"/>
@@ -5229,11 +5229,11 @@
         <v>3</v>
       </c>
       <c r="L49" s="17">
-        <f>B49/K49</f>
+        <f t="shared" si="6"/>
         <v>30.333333333333332</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>93</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>211</v>
       </c>
       <c r="I50" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>35.166666666666664</v>
       </c>
       <c r="J50" s="1"/>
@@ -5264,11 +5264,11 @@
         <v>4</v>
       </c>
       <c r="L50" s="17">
-        <f>B50/K50</f>
+        <f t="shared" si="6"/>
         <v>23.25</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <v>150</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>293</v>
       </c>
       <c r="I51" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>41.857142857142854</v>
       </c>
       <c r="J51" s="1"/>
@@ -5299,11 +5299,11 @@
         <v>5</v>
       </c>
       <c r="L51" s="17">
-        <f>B51/K51</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="2">
         <v>211</v>
       </c>
@@ -5323,11 +5323,11 @@
         <v>6</v>
       </c>
       <c r="L52" s="17">
-        <f>B52/K52</f>
+        <f t="shared" si="6"/>
         <v>35.166666666666664</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>293</v>
       </c>
@@ -5347,11 +5347,11 @@
         <v>7</v>
       </c>
       <c r="L53" s="17">
-        <f>B53/K53</f>
+        <f t="shared" si="6"/>
         <v>41.857142857142854</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>366</v>
       </c>
@@ -5371,11 +5371,11 @@
         <v>8</v>
       </c>
       <c r="L54" s="17">
-        <f>B54/K54</f>
+        <f t="shared" si="6"/>
         <v>45.75</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="2">
         <v>437</v>
       </c>
@@ -5395,11 +5395,11 @@
         <v>9</v>
       </c>
       <c r="L55" s="17">
-        <f>B55/K55</f>
+        <f t="shared" si="6"/>
         <v>48.555555555555557</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
         <v>524</v>
       </c>
@@ -5419,11 +5419,11 @@
         <v>10</v>
       </c>
       <c r="L56" s="17">
-        <f>B56/K56</f>
+        <f t="shared" si="6"/>
         <v>52.4</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
         <v>527</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>546</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="2">
         <v>643</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="2">
         <v>646</v>
       </c>
@@ -5503,8 +5503,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="65" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C65" s="25"/>
       <c r="D65" s="26" t="s">
         <v>248</v>
@@ -5537,7 +5537,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C66" s="29" t="s">
         <v>249</v>
       </c>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="N66" s="23"/>
     </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C67" s="29" t="s">
         <v>250</v>
       </c>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="N67" s="23"/>
     </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C68" s="29" t="s">
         <v>251</v>
       </c>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="N68" s="23"/>
     </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C69" s="29" t="s">
         <v>252</v>
       </c>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="N69" s="23"/>
     </row>
-    <row r="70" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="32" t="s">
         <v>253</v>
       </c>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="N70" s="23"/>
     </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C71" s="38"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -5661,7 +5661,7 @@
       <c r="M71" s="31"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C72" s="29" t="s">
         <v>262</v>
       </c>
@@ -5691,7 +5691,7 @@
       <c r="M72" s="39"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C73" s="29" t="s">
         <v>254</v>
       </c>
@@ -5717,7 +5717,7 @@
       <c r="M73" s="39"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C74" s="29" t="s">
         <v>255</v>
       </c>
@@ -5739,7 +5739,7 @@
       <c r="M74" s="39"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C75" s="29" t="s">
         <v>256</v>
       </c>
@@ -5759,7 +5759,7 @@
       <c r="M75" s="39"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="32" t="s">
         <v>257</v>
       </c>
@@ -5792,7 +5792,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5807,16 +5807,16 @@
       <selection activeCell="O33" sqref="O33:S51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="9.06640625" style="1"/>
+    <col min="1" max="4" width="9.109375" style="1"/>
     <col min="5" max="6" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="3.46484375" customWidth="1"/>
-    <col min="8" max="8" width="3.46484375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.06640625" style="1"/>
+    <col min="7" max="7" width="3.44140625" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>4</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>16.493145036594164</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>18.967116792083292</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>11</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>11</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>12</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>12</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>13</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>14</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>14.558260773112972</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>29</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>31</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>31</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>16.63801231212911</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>33</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>2.9166666666666665</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>34</v>
       </c>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>34</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>36</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>46</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>50</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>50</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>50</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>50</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>52</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>53</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>54</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>16.069706817126736</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>56</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>57</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>60</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>28.121986929971794</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>60</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>61</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>62</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>65</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>66</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>66</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>66</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>3.2777777777777777</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>67</v>
       </c>
@@ -7848,7 +7848,7 @@
       </c>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>68</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>69</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>69</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>69</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>73</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>73</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>73</v>
       </c>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>73</v>
       </c>
@@ -8100,7 +8100,7 @@
       </c>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>73</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>73</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>4.2087542087542085</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>73</v>
       </c>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>74</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>74</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>0.67340067340067333</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>74</v>
       </c>
@@ -8252,7 +8252,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>75</v>
       </c>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>75</v>
       </c>
@@ -8294,7 +8294,7 @@
       </c>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>75</v>
       </c>
@@ -8315,7 +8315,7 @@
       </c>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>75</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>75</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>75</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>75</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>75</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>75</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -8564,7 +8564,7 @@
       </c>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>78</v>
       </c>
@@ -8585,7 +8585,7 @@
       </c>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>79</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>80</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>8.0862533692722369</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>80</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>81</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>83</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>2.6954177897574128</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>83</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>84</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -8848,7 +8848,7 @@
       </c>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -8877,7 +8877,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>84</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>2.2936744282060788</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -8923,7 +8923,7 @@
       </c>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>95</v>
       </c>
@@ -8953,7 +8953,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>95</v>
       </c>
@@ -8996,13 +8996,13 @@
       <selection activeCell="I60" sqref="I60:L85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="9.06640625" style="1"/>
-    <col min="9" max="9" width="9.06640625" style="1"/>
+    <col min="1" max="6" width="9.109375" style="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -9022,7 +9022,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>12</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -9111,7 +9111,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>7.0333333333333332</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>11</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>6.375</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>10</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>14</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>50</v>
       </c>
@@ -9261,7 +9261,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>31</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>75</v>
       </c>
@@ -9321,7 +9321,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -9341,7 +9341,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>75</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>31</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>75</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>25</v>
       </c>
@@ -9461,7 +9461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -9481,7 +9481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>50</v>
       </c>
@@ -9521,7 +9521,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>73</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>75</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>75</v>
       </c>
@@ -9581,7 +9581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>73</v>
       </c>
@@ -9601,7 +9601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>19</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>75</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -9661,7 +9661,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>80</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>75</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>50</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>75</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>75</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>80</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>84</v>
       </c>
@@ -9801,7 +9801,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>67</v>
       </c>
@@ -9821,7 +9821,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>74</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>73</v>
       </c>
@@ -9861,7 +9861,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>73</v>
       </c>
@@ -9881,7 +9881,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>74</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>60</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>95</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>33</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>66</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>95</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>73</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>34</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>73</v>
       </c>
@@ -10061,7 +10061,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>84</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>84</v>
       </c>
@@ -10101,7 +10101,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>84</v>
       </c>
@@ -10121,7 +10121,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>73</v>
       </c>
@@ -10141,7 +10141,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>66</v>
       </c>
@@ -10161,7 +10161,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>60</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>66</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>74</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>54</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>62</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>79</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>29</v>
       </c>
@@ -10340,7 +10340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>68</v>
       </c>
@@ -10372,7 +10372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>65</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>4</v>
       </c>
@@ -10436,7 +10436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -10468,7 +10468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>69</v>
       </c>
@@ -10532,7 +10532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>34</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -10596,7 +10596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>83</v>
       </c>
@@ -10628,7 +10628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>81</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -10692,7 +10692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>87</v>
       </c>
@@ -10724,7 +10724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>36</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>56</v>
       </c>
@@ -10788,7 +10788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>57</v>
       </c>
@@ -10820,7 +10820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>53</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>52</v>
       </c>
@@ -10884,7 +10884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>83</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>21</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>46</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -11012,7 +11012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>78</v>
       </c>
@@ -11044,7 +11044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>61</v>
       </c>
@@ -11076,7 +11076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -11096,7 +11096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>9</v>
       </c>
@@ -11116,7 +11116,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>6</v>
       </c>
@@ -11136,7 +11136,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>6</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>9</v>
       </c>
@@ -11214,12 +11214,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="9.06640625" style="1"/>
+    <col min="1" max="6" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -11239,7 +11239,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>34</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -11279,7 +11279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -11299,7 +11299,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>14</v>
       </c>
@@ -11319,7 +11319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>53</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>56</v>
       </c>
@@ -11359,7 +11359,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>33</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>61</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -11419,7 +11419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -11459,7 +11459,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -11479,7 +11479,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>29</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -11519,7 +11519,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -11559,7 +11559,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -11599,7 +11599,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>78</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>46</v>
       </c>
@@ -11659,7 +11659,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>31</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>65</v>
       </c>
@@ -11699,7 +11699,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>10</v>
       </c>
@@ -11719,7 +11719,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>12</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -11799,7 +11799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>73</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>83</v>
       </c>
@@ -11839,7 +11839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>83</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>69</v>
       </c>
@@ -11879,7 +11879,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>75</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>10</v>
       </c>
@@ -11919,7 +11919,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>87</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>81</v>
       </c>
@@ -11959,7 +11959,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>84</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>84</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>95</v>
       </c>
@@ -12039,7 +12039,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>11</v>
       </c>
@@ -12059,7 +12059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>75</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>50</v>
       </c>
@@ -12099,7 +12099,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>62</v>
       </c>
@@ -12119,7 +12119,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>75</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>75</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>75</v>
       </c>
@@ -12179,7 +12179,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>66</v>
       </c>
@@ -12199,7 +12199,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>69</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>60</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>75</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>66</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>75</v>
       </c>
@@ -12299,7 +12299,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>50</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>73</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>75</v>
       </c>
@@ -12359,7 +12359,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>75</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>75</v>
       </c>
@@ -12399,7 +12399,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>73</v>
       </c>
@@ -12419,7 +12419,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>74</v>
       </c>
@@ -12439,7 +12439,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>66</v>
       </c>
@@ -12479,7 +12479,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>79</v>
       </c>
@@ -12499,7 +12499,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>10</v>
       </c>
@@ -12519,7 +12519,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>50</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>12</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>54</v>
       </c>
@@ -12579,7 +12579,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>84</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>73</v>
       </c>
@@ -12619,7 +12619,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>73</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>12</v>
       </c>
@@ -12659,7 +12659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -12699,7 +12699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>50</v>
       </c>
@@ -12739,7 +12739,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>84</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>60</v>
       </c>
@@ -12779,7 +12779,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>80</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>80</v>
       </c>
@@ -12819,7 +12819,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>68</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>57</v>
       </c>
@@ -12859,7 +12859,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>21</v>
       </c>
@@ -12879,7 +12879,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>67</v>
       </c>
@@ -12899,7 +12899,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>36</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>4</v>
       </c>
@@ -12939,7 +12939,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>31</v>
       </c>
@@ -12959,7 +12959,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>95</v>
       </c>
@@ -12979,7 +12979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>52</v>
       </c>
@@ -12999,7 +12999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>69</v>
       </c>
@@ -13035,14 +13035,14 @@
       <selection activeCell="B70" sqref="B70:D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="9.06640625" style="1"/>
-    <col min="8" max="8" width="9.06640625" style="1"/>
-    <col min="13" max="13" width="9.06640625" style="1"/>
+    <col min="1" max="6" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="13" max="13" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -13062,7 +13062,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>34</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -13135,7 +13135,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -13173,7 +13173,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -13206,7 +13206,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>12</v>
       </c>
@@ -13239,7 +13239,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>33</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -13326,7 +13326,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -13350,7 +13350,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -13417,7 +13417,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>25</v>
       </c>
@@ -13448,7 +13448,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>29</v>
       </c>
@@ -13475,7 +13475,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -13502,7 +13502,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -13529,7 +13529,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -13556,7 +13556,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -13586,7 +13586,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -13616,7 +13616,7 @@
       <c r="K19" s="20"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>75</v>
       </c>
@@ -13646,7 +13646,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -13676,7 +13676,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>75</v>
       </c>
@@ -13706,7 +13706,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>50</v>
       </c>
@@ -13736,7 +13736,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -13763,7 +13763,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>73</v>
       </c>
@@ -13793,7 +13793,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>50</v>
       </c>
@@ -13820,7 +13820,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>75</v>
       </c>
@@ -13847,7 +13847,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>75</v>
       </c>
@@ -13874,7 +13874,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>73</v>
       </c>
@@ -13901,7 +13901,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>75</v>
       </c>
@@ -13931,7 +13931,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>80</v>
       </c>
@@ -13965,7 +13965,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>75</v>
       </c>
@@ -14002,7 +14002,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>50</v>
       </c>
@@ -14039,7 +14039,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>75</v>
       </c>
@@ -14076,7 +14076,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>75</v>
       </c>
@@ -14113,7 +14113,7 @@
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>84</v>
       </c>
@@ -14149,7 +14149,7 @@
         <v>9.5714285714285712</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>80</v>
       </c>
@@ -14172,7 +14172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>74</v>
       </c>
@@ -14195,7 +14195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>73</v>
       </c>
@@ -14218,7 +14218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>73</v>
       </c>
@@ -14241,7 +14241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>74</v>
       </c>
@@ -14264,7 +14264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>60</v>
       </c>
@@ -14287,7 +14287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>95</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>66</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>73</v>
       </c>
@@ -14356,7 +14356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>84</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>84</v>
       </c>
@@ -14402,7 +14402,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>73</v>
       </c>
@@ -14425,7 +14425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>84</v>
       </c>
@@ -14448,7 +14448,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>73</v>
       </c>
@@ -14471,7 +14471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>66</v>
       </c>
@@ -14494,7 +14494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>60</v>
       </c>
@@ -14517,7 +14517,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>66</v>
       </c>
@@ -14540,7 +14540,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>74</v>
       </c>
@@ -14563,7 +14563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>62</v>
       </c>
@@ -14586,7 +14586,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -14609,7 +14609,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>79</v>
       </c>
@@ -14632,7 +14632,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>68</v>
       </c>
@@ -14655,7 +14655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>65</v>
       </c>
@@ -14678,7 +14678,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -14701,7 +14701,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>83</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>69</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>81</v>
       </c>
@@ -14770,7 +14770,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>69</v>
       </c>
@@ -14793,7 +14793,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>87</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>56</v>
       </c>
@@ -14839,7 +14839,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>57</v>
       </c>
@@ -14862,7 +14862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>83</v>
       </c>
@@ -14885,7 +14885,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>78</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>31</v>
       </c>
@@ -14928,7 +14928,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -14948,7 +14948,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>95</v>
       </c>
@@ -14968,7 +14968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>36</v>
       </c>
@@ -14988,7 +14988,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>52</v>
       </c>
@@ -15008,7 +15008,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>11</v>
       </c>
@@ -15028,7 +15028,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>13</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>10</v>
       </c>
@@ -15068,7 +15068,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>14</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>10</v>
       </c>
@@ -15108,7 +15108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -15128,7 +15128,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>34</v>
       </c>
@@ -15148,7 +15148,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>4</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>53</v>
       </c>
@@ -15188,7 +15188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>21</v>
       </c>
@@ -15208,7 +15208,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>46</v>
       </c>
@@ -15228,7 +15228,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>61</v>
       </c>
@@ -15248,7 +15248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -15268,7 +15268,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>9</v>
       </c>
@@ -15305,7 +15305,7 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15320,7 +15320,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15335,9 +15335,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>

</xml_diff>